<commit_message>
Se mejora la forma de obtener las actualizaciones, para no depender del servicio de ASFI
</commit_message>
<xml_diff>
--- a/normativa/Anexos/L01T02C04/L01T02C04A04.xlsx
+++ b/normativa/Anexos/L01T02C04/L01T02C04A04.xlsx
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15:AL16"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2015,9 +2015,9 @@
   <pageSetup scale="96" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Negrita"&amp;8&amp;U
-RECOPILACIÓN DE NORMAS PARA BANCOS Y ENTIDADES FINANCIERAS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
-    <oddFooter>&amp;R&amp;"Times New Roman,Normal"&amp;8Libro 1°
-Título II
+RECOPILACIÓN DE NORMAS PARA SERVICIOS FINANCIEROS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
+    <oddFooter>&amp;R&amp;"Times New Roman,Normal"&amp;8LIBRO 1°
+TÍTULO II
 Capítulo IV
 Anexo 4
 Página 1/1</oddFooter>
@@ -2030,7 +2030,7 @@
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AF2"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3035,7 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3065,7 +3065,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3165,7 +3165,7 @@
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Negrita"&amp;8&amp;U
-RECOPILACIÓN DE NORMAS PARA BANCOS Y ENTIDADES FINANCIERAS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
+RECOPILACIÓN DE NORMAS PARA SERVICIOS FINANCIEROS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
     <oddFooter>&amp;R&amp;"Times New Roman,Normal"&amp;8LIBRO 5°
 TÍTULO I
 Capítulo II

</xml_diff>